<commit_message>
Cambios dispersion separacion bancomer, bug al editar empleado
</commit_message>
<xml_diff>
--- a/Payroll/Content/Download/EjemploLayoutSueldos.xlsx
+++ b/Payroll/Content/Download/EjemploLayoutSueldos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Documents\Proyectos-Raciti\IPSNET-Nomina\devaguilar\Seri\Payroll\Content\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="IPSNet Salario" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Traslado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9666.66 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14666.66 </t>
+  </si>
+  <si>
+    <t>5500.00</t>
   </si>
 </sst>
 </file>
@@ -197,12 +206,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -487,7 +496,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,10 +512,10 @@
       <c r="A1">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -526,7 +535,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>4</v>
       </c>
       <c r="E2">
@@ -535,15 +544,15 @@
       <c r="F2">
         <v>352</v>
       </c>
-      <c r="G2" s="4">
-        <v>5500</v>
-      </c>
-      <c r="H2" s="5">
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4">
         <v>44361</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>4</v>
       </c>
       <c r="E3" s="3">
@@ -552,15 +561,15 @@
       <c r="F3">
         <v>352</v>
       </c>
-      <c r="G3" s="4">
-        <v>14666.666666666668</v>
-      </c>
-      <c r="H3" s="5">
+      <c r="G3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4">
         <v>44361</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>4</v>
       </c>
       <c r="E4" s="3">
@@ -569,15 +578,15 @@
       <c r="F4">
         <v>352</v>
       </c>
-      <c r="G4" s="4">
-        <v>9666.6666666666679</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="G4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4">
         <v>44360</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>5</v>
       </c>
       <c r="E5" s="3">
@@ -586,10 +595,10 @@
       <c r="F5">
         <v>352</v>
       </c>
-      <c r="G5" s="4">
-        <v>9666.6666666666679</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="G5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="4">
         <v>44359</v>
       </c>
     </row>

</xml_diff>